<commit_message>
webapp2 works with second page
</commit_message>
<xml_diff>
--- a/data/Data_Model.xlsx
+++ b/data/Data_Model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\Documents\Webapp\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{527A268A-B7E9-4776-AF2C-FFA5C516C607}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4592F7F-3DBC-4BE2-BB76-6FE27E36453C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="-90" yWindow="120" windowWidth="24180" windowHeight="15250" activeTab="1" xr2:uid="{2A577089-14E3-46C5-B0F5-6C47B76D92C7}"/>
+    <workbookView xWindow="2685" yWindow="2685" windowWidth="28800" windowHeight="15225" activeTab="1" xr2:uid="{2A577089-14E3-46C5-B0F5-6C47B76D92C7}"/>
   </bookViews>
   <sheets>
     <sheet name="weather forecast" sheetId="1" r:id="rId1"/>
@@ -280,9 +280,6 @@
     <t>International Energy Agency</t>
   </si>
   <si>
-    <t>Very high spatial (6 km) and temporal (1 hour) resolution, 1995 to 2016, 1 file of 1.5 GB per month, curvilinear map --&gt; requires coordinate transformation, 01/1995 - 08/2019</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://www.iea.org/data-and-statistics/data-product/renewables-information </t>
   </si>
   <si>
@@ -394,9 +391,6 @@
     <t>no (latest version 2018)</t>
   </si>
   <si>
-    <t>1940 - present, simple, because 100 m u and v component selectable (https://cds.climate.copernicus.eu/datasets/reanalysis-era5-single-levels?tab=download) as used in forecast, sub-region extraction available, download or API available (request required, e. g. for API key required)</t>
-  </si>
-  <si>
     <t>at WPP level, but data only for windparks &gt; 100 MW ("Actual net generation output (MW) per market time unit and per generation unit of 100 MW or more installed generation capacity."), exportable with FTP Client software FileZilla (https://transparency.entsoe.eu/content/static_content/Static%20content/knowledge%20base/SFTP-Transparency_Docs.html, Hostname: sftp-transparency.entsoe.eu, Port: 22), 12/2014 - present,
 only countries uploading wind energy data are 01/2015: BE, DK, GB. 06/2019: BE, DK, GB. 10/2024: BE, DK, FR, IT</t>
   </si>
@@ -444,6 +438,12 @@
   </si>
   <si>
     <t>for yaw, pitch, stall control, WPPs measure wind speed and direction --&gt; difficult ot obtain, not required, because good weather data available, not useful, because arbitrary locations should be selectable, formerly sensors behind nacelles --&gt; lower wind speed</t>
+  </si>
+  <si>
+    <t>Very high spatial (6 km) and temporal (1 hour) resolution, 1995 to 2016, 1 file of 1.5 GB per month, curvilinear map --&gt; requires coordinate transformation, 01/1995 - 08/2019, spatial resolution: 6 km x 6 km, temporal resolution: hourly</t>
+  </si>
+  <si>
+    <t>1940 - present, simple, because 100 m u and v component selectable (https://cds.climate.copernicus.eu/datasets/reanalysis-era5-single-levels?tab=download) as used in forecast, sub-region extraction available, download or API available (request required, e. g. for API key required), spatial resolution: 31 km x 31 km, temporal resolution: hourly</t>
   </si>
 </sst>
 </file>
@@ -564,7 +564,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1223,7 +1223,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1253,10 +1253,10 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>14</v>
       </c>
@@ -1270,13 +1270,13 @@
         <v>39</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>58</v>
+        <v>107</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>11</v>
       </c>
@@ -1290,10 +1290,10 @@
         <v>37</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1311,7 +1311,7 @@
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1328,21 +1328,21 @@
         <v>37</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F6" s="1"/>
     </row>
@@ -1396,13 +1396,13 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>33</v>
@@ -1416,7 +1416,7 @@
         <v>16</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>5</v>
@@ -1425,19 +1425,19 @@
         <v>18</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>37</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1454,20 +1454,20 @@
         <v>21</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2" t="s">
         <v>37</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -1475,22 +1475,22 @@
         <v>22</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>37</v>
@@ -1510,10 +1510,10 @@
         <v>5</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -1535,16 +1535,16 @@
         <v>5</v>
       </c>
       <c r="D6" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>77</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>37</v>
@@ -1565,20 +1565,20 @@
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>34</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1592,13 +1592,13 @@
         <v>5</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>35</v>
@@ -1618,10 +1618,10 @@
         <v>5</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>36</v>
@@ -1632,7 +1632,7 @@
     </row>
     <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>49</v>
@@ -1641,13 +1641,13 @@
         <v>6</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>37</v>
@@ -1658,25 +1658,25 @@
     </row>
     <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="I11" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1746,7 +1746,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>39</v>
@@ -1757,13 +1757,13 @@
         <v>57</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>37</v>
@@ -1814,16 +1814,16 @@
     </row>
     <row r="2" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>106</v>
-      </c>
       <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1871,16 +1871,16 @@
     </row>
     <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>37</v>
@@ -1888,13 +1888,13 @@
     </row>
     <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>37</v>
@@ -1902,16 +1902,16 @@
     </row>
     <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>83</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>37</v>

</xml_diff>

<commit_message>
MLP and LSTM model, updated webapp2
</commit_message>
<xml_diff>
--- a/data/Data_Model.xlsx
+++ b/data/Data_Model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\Documents\Webapp\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FEDC39A-E167-4E12-B5EE-741E96A18124}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B05C57BF-C754-4D90-B4C0-25B7F68955EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="24220" windowHeight="15500" activeTab="3" xr2:uid="{2A577089-14E3-46C5-B0F5-6C47B76D92C7}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="24220" windowHeight="15500" xr2:uid="{2A577089-14E3-46C5-B0F5-6C47B76D92C7}"/>
   </bookViews>
   <sheets>
     <sheet name="weather forecast" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="121">
   <si>
     <t>ECMWF</t>
   </si>
@@ -437,9 +437,6 @@
     <t>data from WPP sensors</t>
   </si>
   <si>
-    <t>for yaw, pitch, stall control, WPPs measure wind speed and direction --&gt; difficult ot obtain, not required, because good weather data available, not useful, because arbitrary locations should be selectable, formerly sensors behind nacelles --&gt; lower wind speed</t>
-  </si>
-  <si>
     <t>1940 - present, simple, because 100 m u and v component selectable (https://cds.climate.copernicus.eu/datasets/reanalysis-era5-single-levels?tab=download) as used in forecast, sub-region extraction available, download or API available (request required, e. g. for API key required), spatial resolution: 31 km x 31 km, temporal resolution: hourly</t>
   </si>
   <si>
@@ -462,6 +459,27 @@
   </si>
   <si>
     <t xml:space="preserve">https://opendata.dwd.de/climate_environment/REA/COSMO_REA6/hourly/2D/PS/ </t>
+  </si>
+  <si>
+    <t>https://www.eex-transparency.com/power/de/production/usage</t>
+  </si>
+  <si>
+    <t>"Power Production per Unit", not accessible with bulk download or API, no additional power plant information, not even location, only for a very small past time period</t>
+  </si>
+  <si>
+    <t>EEX Transparency Platform</t>
+  </si>
+  <si>
+    <t>Eurostag</t>
+  </si>
+  <si>
+    <t>not at WPP level, only at country lvel; monthly aggregated</t>
+  </si>
+  <si>
+    <t>https://ec.europa.eu/eurostat/de/data/database</t>
+  </si>
+  <si>
+    <t>for yaw, pitch, stall control, WPPs measure wind speed and direction --&gt; difficult ot obtain, not required, because good weather data available, not useful, because arbitrary locations should be selectable, formerly sensors behind nacelles --&gt; lower wind speed, existence of these data confirmed in [MAR2018]</t>
   </si>
 </sst>
 </file>
@@ -635,15 +653,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i/>
@@ -660,6 +669,15 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -771,55 +789,55 @@
     <tableColumn id="4" xr3:uid="{A365E008-1A8F-40FA-A9F4-EDBEF77C474C}" name="Area" dataDxfId="30"/>
     <tableColumn id="5" xr3:uid="{8DDE3FAB-CEAF-4DFA-93F0-0A311F6751AC}" name="Description" dataDxfId="29"/>
     <tableColumn id="6" xr3:uid="{3740D99D-889E-48CC-BF8B-5D272FDB37B0}" name="Creator" dataDxfId="28"/>
-    <tableColumn id="7" xr3:uid="{82FD5AA3-299B-40D2-B9CB-39F3BA98F999}" name="wind speed" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{847A8843-BE43-4A20-919C-C035AD03837E}" name="temperature" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{1339EAEB-A298-4B0F-9595-87879A755CD8}" name="pressure" dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{82FD5AA3-299B-40D2-B9CB-39F3BA98F999}" name="wind speed" dataDxfId="27"/>
+    <tableColumn id="8" xr3:uid="{847A8843-BE43-4A20-919C-C035AD03837E}" name="temperature" dataDxfId="26"/>
+    <tableColumn id="9" xr3:uid="{1339EAEB-A298-4B0F-9595-87879A755CD8}" name="pressure" dataDxfId="25"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{BC444647-8C5A-4014-AE07-133383825030}" name="Table5" displayName="Table5" ref="A1:I11" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{BC444647-8C5A-4014-AE07-133383825030}" name="Table5" displayName="Table5" ref="A1:I11" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
   <autoFilter ref="A1:I11" xr:uid="{BC444647-8C5A-4014-AE07-133383825030}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{C6DB6FE3-7CF0-41B4-8837-8EE64269A96A}" name="Provider" dataDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{C2C7D0D7-2E6E-410A-B5D9-AA0B558DFCDB}" name="Link" dataDxfId="24" dataCellStyle="Hyperlink"/>
-    <tableColumn id="3" xr3:uid="{45957BE7-F087-469E-9D47-F7479C615DA7}" name="Costs" dataDxfId="23"/>
-    <tableColumn id="4" xr3:uid="{894D8DA0-597B-4F85-AA9A-BF5B1496AED1}" name="Description" dataDxfId="22"/>
-    <tableColumn id="5" xr3:uid="{2978BF80-BC4F-404A-986E-EB778660ABF0}" name="with technical specifications (apart capacity)?" dataDxfId="21"/>
-    <tableColumn id="6" xr3:uid="{FE2FC897-3B75-41CF-9127-E40412D7EF33}" name="updated / maintained?" dataDxfId="20"/>
-    <tableColumn id="7" xr3:uid="{CB23B69B-DCC8-4DCA-9CB8-EA96E32FC86B}" name="validated / not public?" dataDxfId="19"/>
-    <tableColumn id="8" xr3:uid="{691D97FA-AEAB-450E-8C34-876FB1F92E8B}" name="area" dataDxfId="18"/>
-    <tableColumn id="9" xr3:uid="{7C588C0F-B30F-4B28-9DBA-196BD6009E77}" name="matching parameters (ID, coordinates) (italic: proprietary Ids)" dataDxfId="17"/>
+    <tableColumn id="1" xr3:uid="{C6DB6FE3-7CF0-41B4-8837-8EE64269A96A}" name="Provider" dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{C2C7D0D7-2E6E-410A-B5D9-AA0B558DFCDB}" name="Link" dataDxfId="21" dataCellStyle="Hyperlink"/>
+    <tableColumn id="3" xr3:uid="{45957BE7-F087-469E-9D47-F7479C615DA7}" name="Costs" dataDxfId="20"/>
+    <tableColumn id="4" xr3:uid="{894D8DA0-597B-4F85-AA9A-BF5B1496AED1}" name="Description" dataDxfId="19"/>
+    <tableColumn id="5" xr3:uid="{2978BF80-BC4F-404A-986E-EB778660ABF0}" name="with technical specifications (apart capacity)?" dataDxfId="18"/>
+    <tableColumn id="6" xr3:uid="{FE2FC897-3B75-41CF-9127-E40412D7EF33}" name="updated / maintained?" dataDxfId="17"/>
+    <tableColumn id="7" xr3:uid="{CB23B69B-DCC8-4DCA-9CB8-EA96E32FC86B}" name="validated / not public?" dataDxfId="16"/>
+    <tableColumn id="8" xr3:uid="{691D97FA-AEAB-450E-8C34-876FB1F92E8B}" name="area" dataDxfId="15"/>
+    <tableColumn id="9" xr3:uid="{7C588C0F-B30F-4B28-9DBA-196BD6009E77}" name="matching parameters (ID, coordinates) (italic: proprietary Ids)" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1F3C284E-2D9E-463F-9F2A-6E84937AD136}" name="Table3" displayName="Table3" ref="A1:E3" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
-  <autoFilter ref="A1:E3" xr:uid="{1F3C284E-2D9E-463F-9F2A-6E84937AD136}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1F3C284E-2D9E-463F-9F2A-6E84937AD136}" name="Table3" displayName="Table3" ref="A1:E5" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+  <autoFilter ref="A1:E5" xr:uid="{1F3C284E-2D9E-463F-9F2A-6E84937AD136}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{3F0D1124-066B-4E3A-A294-E460F30767AF}" name="Provider" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{A7805D07-626E-49E5-8032-3716B8C697BB}" name="Link" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{567AE5C4-1E24-4909-8FB3-954AEDB7D138}" name="Costs" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{A80B67ED-EB26-40FB-BD44-C497686319AF}" name="Description" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{8651FCB4-E138-4F7B-B8BE-4DCB18BF623B}" name="area" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{3F0D1124-066B-4E3A-A294-E460F30767AF}" name="Provider" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{A7805D07-626E-49E5-8032-3716B8C697BB}" name="Link" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{567AE5C4-1E24-4909-8FB3-954AEDB7D138}" name="Costs" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{A80B67ED-EB26-40FB-BD44-C497686319AF}" name="Description" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{8651FCB4-E138-4F7B-B8BE-4DCB18BF623B}" name="area" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{9F9C695A-1B5B-410C-9DC4-82A5FE910542}" name="Table4" displayName="Table4" ref="A1:E4" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{9F9C695A-1B5B-410C-9DC4-82A5FE910542}" name="Table4" displayName="Table4" ref="A1:E4" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
   <autoFilter ref="A1:E4" xr:uid="{9F9C695A-1B5B-410C-9DC4-82A5FE910542}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{1D4A4FEF-BBEE-4F48-9578-49BD0251EFA7}" name="Provider" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{142F0DEB-E26B-40A1-BB89-BE76E869D9EF}" name="Link" dataDxfId="6" dataCellStyle="Hyperlink"/>
-    <tableColumn id="3" xr3:uid="{CCCE6F29-3203-4C95-B925-4AB3CE399E5B}" name="Costs" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{3A25A516-50A1-4ED0-B7A3-6624422041B3}" name="Description" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{29A983F8-3F1D-4082-9FC4-CE78E5963EDB}" name="area" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{1D4A4FEF-BBEE-4F48-9578-49BD0251EFA7}" name="Provider" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{142F0DEB-E26B-40A1-BB89-BE76E869D9EF}" name="Link" dataDxfId="3" dataCellStyle="Hyperlink"/>
+    <tableColumn id="3" xr3:uid="{CCCE6F29-3203-4C95-B925-4AB3CE399E5B}" name="Costs" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{3A25A516-50A1-4ED0-B7A3-6624422041B3}" name="Description" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{29A983F8-3F1D-4082-9FC4-CE78E5963EDB}" name="area" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1144,19 +1162,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03DA9FC3-3033-41B6-8D50-FCDEBAA0FA29}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
-    <col min="2" max="2" width="44.85546875" customWidth="1"/>
+    <col min="2" max="2" width="44.81640625" customWidth="1"/>
     <col min="4" max="4" width="28" customWidth="1"/>
-    <col min="5" max="5" width="65.140625" customWidth="1"/>
+    <col min="5" max="5" width="65.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1173,7 +1191,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -1190,7 +1208,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>45</v>
       </c>
@@ -1205,7 +1223,7 @@
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -1218,7 +1236,7 @@
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -1253,23 +1271,23 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" customWidth="1"/>
-    <col min="2" max="2" width="33.140625" customWidth="1"/>
+    <col min="1" max="1" width="15.453125" customWidth="1"/>
+    <col min="2" max="2" width="33.1796875" customWidth="1"/>
     <col min="3" max="3" width="7" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" customWidth="1"/>
-    <col min="5" max="5" width="62.28515625" customWidth="1"/>
+    <col min="4" max="4" width="11.453125" customWidth="1"/>
+    <col min="5" max="5" width="62.26953125" customWidth="1"/>
     <col min="6" max="6" width="43" customWidth="1"/>
-    <col min="7" max="7" width="17.7109375" customWidth="1"/>
-    <col min="8" max="8" width="16.5703125" customWidth="1"/>
-    <col min="9" max="9" width="18.5703125" customWidth="1"/>
+    <col min="7" max="7" width="17.7265625" customWidth="1"/>
+    <col min="8" max="8" width="16.54296875" customWidth="1"/>
+    <col min="9" max="9" width="18.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1289,21 +1307,21 @@
         <v>99</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>5</v>
@@ -1312,7 +1330,7 @@
         <v>39</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>95</v>
@@ -1321,13 +1339,13 @@
         <v>15</v>
       </c>
       <c r="H2" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>11</v>
       </c>
@@ -1341,7 +1359,7 @@
         <v>37</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>96</v>
@@ -1350,7 +1368,7 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -1371,7 +1389,7 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -1394,7 +1412,7 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>105</v>
       </c>
@@ -1402,7 +1420,7 @@
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
-        <v>106</v>
+        <v>120</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
@@ -1430,24 +1448,24 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView zoomScale="70" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="28.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="39.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="1"/>
-    <col min="4" max="4" width="56.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="29.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="23.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="28.1796875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="39.26953125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.1796875" style="1"/>
+    <col min="4" max="4" width="56.54296875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="29.54296875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="23.1796875" style="1" customWidth="1"/>
     <col min="7" max="7" width="48" style="1" customWidth="1"/>
-    <col min="8" max="8" width="25.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="25.1796875" style="1" customWidth="1"/>
     <col min="9" max="9" width="89" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="1"/>
+    <col min="10" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1476,7 +1494,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>16</v>
       </c>
@@ -1505,7 +1523,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>19</v>
       </c>
@@ -1535,7 +1553,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="87" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>22</v>
       </c>
@@ -1564,7 +1582,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
@@ -1589,7 +1607,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>25</v>
       </c>
@@ -1618,7 +1636,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="87" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>28</v>
       </c>
@@ -1646,7 +1664,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>30</v>
       </c>
@@ -1672,7 +1690,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>32</v>
       </c>
@@ -1695,7 +1713,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>74</v>
       </c>
@@ -1721,7 +1739,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>84</v>
       </c>
@@ -1767,23 +1785,23 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C401C7E-DA12-4B53-A03F-4F3FE27EAC06}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="27" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="1"/>
-    <col min="4" max="4" width="193.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="31.1796875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.1796875" style="1"/>
+    <col min="4" max="4" width="193.81640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1796875" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1800,7 +1818,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>55</v>
       </c>
@@ -1817,7 +1835,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>57</v>
       </c>
@@ -1832,6 +1850,40 @@
       </c>
       <c r="E3" s="1" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1854,15 +1906,15 @@
       <selection activeCell="D2" sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" customWidth="1"/>
-    <col min="3" max="3" width="8.5703125" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" customWidth="1"/>
+    <col min="1" max="1" width="18.81640625" customWidth="1"/>
+    <col min="2" max="2" width="17.453125" customWidth="1"/>
+    <col min="3" max="3" width="8.54296875" customWidth="1"/>
+    <col min="4" max="4" width="22.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>1</v>
       </c>
@@ -1877,7 +1929,7 @@
       </c>
       <c r="E1" s="9"/>
     </row>
-    <row r="2" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>102</v>
       </c>
@@ -1907,17 +1959,17 @@
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="42.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="1"/>
-    <col min="4" max="4" width="121.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="18.26953125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="42.7265625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.1796875" style="1"/>
+    <col min="4" max="4" width="121.54296875" style="1" customWidth="1"/>
     <col min="5" max="5" width="10" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="6" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1934,7 +1986,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>60</v>
       </c>
@@ -1951,7 +2003,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>63</v>
       </c>
@@ -1965,7 +2017,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>81</v>
       </c>

</xml_diff>

<commit_message>
combined WPP data and production
</commit_message>
<xml_diff>
--- a/data/Data_Model.xlsx
+++ b/data/Data_Model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\Documents\Webapp\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24952B7E-0E10-4411-BB23-B5E2554CD8B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE8E516A-2146-4CE9-BA86-E2A8753C64F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="990" windowWidth="23980" windowHeight="15010" activeTab="3" xr2:uid="{2A577089-14E3-46C5-B0F5-6C47B76D92C7}"/>
+    <workbookView xWindow="11910" yWindow="0" windowWidth="12180" windowHeight="15370" activeTab="1" xr2:uid="{2A577089-14E3-46C5-B0F5-6C47B76D92C7}"/>
   </bookViews>
   <sheets>
     <sheet name="weather forecast" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="115">
   <si>
     <t>ECMWF</t>
   </si>
@@ -437,24 +437,6 @@
   </si>
   <si>
     <t>Very high spatial (6 km) and temporal (1 hour) resolution, 1995 to 2016, 1 file of 1.5 GB per month, curvilinear map --&gt; requires coordinate transformation, 01/1995 - 08/2019, spatial resolution: 6 km x 6 km, temporal resolution: hourly; T_2M is 2 m temperature, WS_100 is wind speed in 100 m, ps is not reduced surface pressure</t>
-  </si>
-  <si>
-    <t>https://opendata.dwd.de/climate_environment/REA/</t>
-  </si>
-  <si>
-    <t>temperature</t>
-  </si>
-  <si>
-    <t>wind speed</t>
-  </si>
-  <si>
-    <t>pressure</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://opendata.dwd.de/climate_environment/REA/COSMO_REA6/hourly/2D/T_2M/ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://opendata.dwd.de/climate_environment/REA/COSMO_REA6/hourly/2D/PS/ </t>
   </si>
   <si>
     <t>https://www.eex-transparency.com/power/de/production/usage</t>
@@ -586,7 +568,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -613,13 +595,16 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="42">
+  <dxfs count="39">
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -753,15 +738,6 @@
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -776,32 +752,29 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{4F12E0D7-3F7A-4487-8316-91D8EC14F3DE}" name="Table7" displayName="Table7" ref="A1:E5" totalsRowShown="0" dataDxfId="41">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{4F12E0D7-3F7A-4487-8316-91D8EC14F3DE}" name="Table7" displayName="Table7" ref="A1:E5" totalsRowShown="0" dataDxfId="38">
   <autoFilter ref="A1:E5" xr:uid="{4F12E0D7-3F7A-4487-8316-91D8EC14F3DE}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{763B3611-6A05-4496-9549-28A9C3FF5F24}" name="Provider" dataDxfId="40"/>
-    <tableColumn id="2" xr3:uid="{DEB2246F-248B-49E0-9C7A-770975C5608B}" name="Link" dataDxfId="39" dataCellStyle="Hyperlink"/>
-    <tableColumn id="3" xr3:uid="{09CDAAEA-1CF4-4A9A-A8FC-9A9CF0E41FB1}" name="Costs" dataDxfId="38"/>
-    <tableColumn id="4" xr3:uid="{FE1B169A-0800-46A4-813B-6C6FDE081AA2}" name="Area" dataDxfId="37"/>
-    <tableColumn id="5" xr3:uid="{3AEBE993-BA1D-4FC9-A845-588AF4BDBC18}" name="Description" dataDxfId="36"/>
+    <tableColumn id="1" xr3:uid="{763B3611-6A05-4496-9549-28A9C3FF5F24}" name="Provider" dataDxfId="37"/>
+    <tableColumn id="2" xr3:uid="{DEB2246F-248B-49E0-9C7A-770975C5608B}" name="Link" dataDxfId="36" dataCellStyle="Hyperlink"/>
+    <tableColumn id="3" xr3:uid="{09CDAAEA-1CF4-4A9A-A8FC-9A9CF0E41FB1}" name="Costs" dataDxfId="35"/>
+    <tableColumn id="4" xr3:uid="{FE1B169A-0800-46A4-813B-6C6FDE081AA2}" name="Area" dataDxfId="34"/>
+    <tableColumn id="5" xr3:uid="{3AEBE993-BA1D-4FC9-A845-588AF4BDBC18}" name="Description" dataDxfId="33"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D2EAB288-5B2A-41B1-8B80-D0AD72606228}" name="Table6" displayName="Table6" ref="A1:I6" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
-  <autoFilter ref="A1:I6" xr:uid="{D2EAB288-5B2A-41B1-8B80-D0AD72606228}"/>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{A15C01DA-CA22-47E7-B80F-E804FFA3B0A3}" name="Provider" dataDxfId="33"/>
-    <tableColumn id="2" xr3:uid="{EBCD32C8-5E9A-42BD-9633-EC1421AA1D88}" name="Link" dataDxfId="32" dataCellStyle="Hyperlink"/>
-    <tableColumn id="3" xr3:uid="{A8CFEFEC-060D-4296-A172-5F2F67680987}" name="Costs" dataDxfId="31"/>
-    <tableColumn id="4" xr3:uid="{A365E008-1A8F-40FA-A9F4-EDBEF77C474C}" name="Area" dataDxfId="30"/>
-    <tableColumn id="5" xr3:uid="{8DDE3FAB-CEAF-4DFA-93F0-0A311F6751AC}" name="Description" dataDxfId="29"/>
-    <tableColumn id="6" xr3:uid="{3740D99D-889E-48CC-BF8B-5D272FDB37B0}" name="Creator" dataDxfId="28"/>
-    <tableColumn id="7" xr3:uid="{82FD5AA3-299B-40D2-B9CB-39F3BA98F999}" name="wind speed" dataDxfId="27"/>
-    <tableColumn id="8" xr3:uid="{847A8843-BE43-4A20-919C-C035AD03837E}" name="temperature" dataDxfId="26"/>
-    <tableColumn id="9" xr3:uid="{1339EAEB-A298-4B0F-9595-87879A755CD8}" name="pressure" dataDxfId="25"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D2EAB288-5B2A-41B1-8B80-D0AD72606228}" name="Table6" displayName="Table6" ref="A1:F6" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
+  <autoFilter ref="A1:F6" xr:uid="{D2EAB288-5B2A-41B1-8B80-D0AD72606228}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{A15C01DA-CA22-47E7-B80F-E804FFA3B0A3}" name="Provider" dataDxfId="30"/>
+    <tableColumn id="2" xr3:uid="{EBCD32C8-5E9A-42BD-9633-EC1421AA1D88}" name="Link" dataDxfId="29" dataCellStyle="Hyperlink"/>
+    <tableColumn id="3" xr3:uid="{A8CFEFEC-060D-4296-A172-5F2F67680987}" name="Costs" dataDxfId="28"/>
+    <tableColumn id="4" xr3:uid="{A365E008-1A8F-40FA-A9F4-EDBEF77C474C}" name="Area" dataDxfId="27"/>
+    <tableColumn id="5" xr3:uid="{8DDE3FAB-CEAF-4DFA-93F0-0A311F6751AC}" name="Description" dataDxfId="26"/>
+    <tableColumn id="6" xr3:uid="{3740D99D-889E-48CC-BF8B-5D272FDB37B0}" name="Creator" dataDxfId="25"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1278,10 +1251,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B86138A-D965-4750-B9A0-F620EAFBC54F}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1297,7 +1270,7 @@
     <col min="9" max="9" width="18.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1316,22 +1289,13 @@
       <c r="F1" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
+    </row>
+    <row r="2" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="10" t="s">
         <v>14</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>107</v>
+        <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>5</v>
@@ -1345,17 +1309,8 @@
       <c r="F2" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>11</v>
       </c>
@@ -1374,11 +1329,8 @@
       <c r="F3" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -1395,11 +1347,8 @@
       <c r="F4" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-    </row>
-    <row r="5" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -1418,11 +1367,8 @@
       <c r="F5" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-    </row>
-    <row r="6" spans="1:9" ht="217.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:6" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>104</v>
       </c>
@@ -1430,25 +1376,20 @@
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" xr:uid="{5AB59A48-E9C0-4612-B80D-DF91AC321927}"/>
     <hyperlink ref="B4" r:id="rId2" xr:uid="{D705CCB2-FA26-47B3-AC56-16EB0A772224}"/>
     <hyperlink ref="B5" r:id="rId3" xr:uid="{0DB67E33-255F-404A-B545-E9BE58AC0ACB}"/>
-    <hyperlink ref="G2" r:id="rId4" xr:uid="{E584F813-AB09-4A3B-A8FE-F8315B7E9F42}"/>
-    <hyperlink ref="H2" r:id="rId5" xr:uid="{E6FCFA98-1E81-43BD-A5E2-01DD9ED90DB8}"/>
-    <hyperlink ref="I2" r:id="rId6" xr:uid="{931F0448-216F-482A-9D1B-D59C42A78A86}"/>
+    <hyperlink ref="B2" r:id="rId4" xr:uid="{E3C23749-AAFA-49ED-B8CA-511CCC8986C4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1797,7 +1738,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C401C7E-DA12-4B53-A03F-4F3FE27EAC06}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -1839,7 +1780,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>39</v>
@@ -1864,16 +1805,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>39</v>
@@ -1881,16 +1822,16 @@
     </row>
     <row r="5" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
json, times for production
</commit_message>
<xml_diff>
--- a/data/Data_Model.xlsx
+++ b/data/Data_Model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\Documents\Webapp\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE8E516A-2146-4CE9-BA86-E2A8753C64F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06453585-B795-4F58-89B9-FA18E7448F74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11910" yWindow="0" windowWidth="12180" windowHeight="15370" activeTab="1" xr2:uid="{2A577089-14E3-46C5-B0F5-6C47B76D92C7}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="24220" windowHeight="15500" activeTab="1" xr2:uid="{2A577089-14E3-46C5-B0F5-6C47B76D92C7}"/>
   </bookViews>
   <sheets>
     <sheet name="weather forecast" sheetId="1" r:id="rId1"/>
@@ -568,7 +568,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -593,9 +593,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1254,7 +1251,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1291,7 +1288,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B2" s="3" t="s">

</xml_diff>